<commit_message>
ZSS-807: fine tune test case.
</commit_message>
<xml_diff>
--- a/zss.test/src/main/webapp/issue3/book/807-documentLink.xlsx
+++ b/zss.test/src/main/webapp/issue3/book/807-documentLink.xlsx
@@ -13,8 +13,10 @@
     <sheet name="Sheet4" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="AFormula">SUM(1,2)</definedName>
     <definedName name="Applicant">main!#REF!</definedName>
     <definedName name="From">main!#REF!</definedName>
+    <definedName name="InSheetName" localSheetId="1">main!$E$12</definedName>
     <definedName name="MainC4_D5">main!$C$4:$D$5</definedName>
     <definedName name="Reason">main!#REF!</definedName>
     <definedName name="RequestDate">main!#REF!</definedName>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Go to sheet 2</t>
   </si>
@@ -46,6 +48,12 @@
   </si>
   <si>
     <t>Go to sheet 4</t>
+  </si>
+  <si>
+    <t>Sheet''s 2'!InSheetName</t>
+  </si>
+  <si>
+    <t>main!A1</t>
   </si>
 </sst>
 </file>
@@ -109,11 +117,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -418,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C1:G1"/>
+  <dimension ref="C1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -450,12 +464,24 @@
         <v>4</v>
       </c>
     </row>
+    <row r="8" spans="3:7">
+      <c r="C8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7">
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C1" location="Sheet2!A2" display="Go to sheet 2"/>
     <hyperlink ref="E1" location="Sheet3!A4" display="Go to sheet 3"/>
     <hyperlink ref="G1" location="Sheet4!A1" display="Go to sheet 4"/>
+    <hyperlink ref="C8" location="'Sheet''s 2'!InSheetName" display="'Sheet''s 2'!InSheetName"/>
+    <hyperlink ref="E11" location="main!A1" display="main!A1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
@@ -472,7 +498,7 @@
   <dimension ref="B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>

</xml_diff>